<commit_message>
Update generate_answers.py to change key from "_id" to "id" in node_data mapping
</commit_message>
<xml_diff>
--- a/oncopro/oncopro_questions.xlsx
+++ b/oncopro/oncopro_questions.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Old" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,12 +12,177 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
   <si>
     <t>question_en</t>
   </si>
   <si>
     <t>question_de</t>
+  </si>
+  <si>
+    <t>What factors are considered to determine T-stage for head and neck cancers?</t>
+  </si>
+  <si>
+    <t>Was wird zur Bestimmung des T-Stadiums bei Kopf-Hals-Tumoren berücksichtigt?</t>
+  </si>
+  <si>
+    <t>What criteria are used to assess regional lymph nodes ivolvement (N-stage) in head and neck cancers?</t>
+  </si>
+  <si>
+    <t>Welche Kriterien werden zur Beurteilung der Beteiligung regionaler Lymphknoten (N-Stadium) bei Kopf-Hals-Tumoren verwendet?</t>
+  </si>
+  <si>
+    <t>How does tumor size, location and spread influence the stage of head and neck cancers?</t>
+  </si>
+  <si>
+    <t>Wie beeinflussen Tumorgröße, Lokalisation und Ausbreitung das Stadium von Kopf-Hals-Tumoren?</t>
+  </si>
+  <si>
+    <t>Are there specific biomarkers or genetic factors used in staging head and neck cancers?</t>
+  </si>
+  <si>
+    <t>Gibt es spezifische Biomarker oder genetische Faktoren, die für das Staging von Kopf-Hals-Tumoren verwendet werden?</t>
+  </si>
+  <si>
+    <t>How is the overall stage assigned in head and neck cancers and what are the factors involved in each stage?</t>
+  </si>
+  <si>
+    <t>Wie wird das Gesamtstadium bei Kopf-Hals-Tumoren zugewiesen, und welche Faktoren fließen in die einzelnen Stadien ein?</t>
+  </si>
+  <si>
+    <t>What are the first-line treatment options for laryngeal carcinoma based on stage of the disease?</t>
+  </si>
+  <si>
+    <t>Was sind die Erstlinien-Behandlungsoptionen für das Larynxkarzinom je nach Krankheitsstadium?</t>
+  </si>
+  <si>
+    <t>When is radiation therapy typically used in the treatment of laryngeal carcinoma?</t>
+  </si>
+  <si>
+    <t>Wann wird die Strahlentherapie typischerweise bei der Behandlung des Larynxkarzinoms eingesetzt?</t>
+  </si>
+  <si>
+    <t>What are the potential surgical procedures (e.g. partial larynectomy vs. total laryngectomy)?</t>
+  </si>
+  <si>
+    <t>Welche operativen Verfahren kommen infrage (z. B. partielle Laryngektomie vs. totale Laryngektomie)?</t>
+  </si>
+  <si>
+    <t>What chemotherapy is used in treating laryngeal carcinoma?</t>
+  </si>
+  <si>
+    <t>Welche Chemotherapie wird bei der Behandlung des Larynxkarzinoms eingesetzt?</t>
+  </si>
+  <si>
+    <t>Are there any targeted therapies or immuntherapies currently recommended for laryngeal carcinoma?</t>
+  </si>
+  <si>
+    <t>Gibt es derzeit empfohlene zielgerichtete Therapien oder Immuntherapien für das Larynxkarzinom?</t>
+  </si>
+  <si>
+    <t>What factors influence the choice of adjuvant treatment?</t>
+  </si>
+  <si>
+    <t>Welche Faktoren beeinflussen die Wahl der adjuvanten Therapie?</t>
+  </si>
+  <si>
+    <t>What are the current recommendations for the treatment of early stage cervical cancer (stages I and II)?</t>
+  </si>
+  <si>
+    <t>Was sind die aktuellen Empfehlungen für die Behandlung des Zervixkarzinoms im Frühstadium (Stadien I und II)?</t>
+  </si>
+  <si>
+    <t>How is advanced-staged cervical cancer (stages III and IV) typically treated according to the latest guidelines?</t>
+  </si>
+  <si>
+    <t>Wie wird das fortgeschrittene Zervixkarzinom (Stadien III und IV) gemäß den neuesten Leitlinien typischerweise behandelt?</t>
+  </si>
+  <si>
+    <t>When is radation therapy recommended ?</t>
+  </si>
+  <si>
+    <t>Wann wird eine Strahlentherapie empfohlen?</t>
+  </si>
+  <si>
+    <t>What are the follow-up care guidelines ater treatment for cervical cancer to monitor for recurrence?</t>
+  </si>
+  <si>
+    <t>Welche Nachsorgeempfehlungen gibt es nach der Behandlung des Zervixkarzinoms zur Überwachung auf ein Rezidiv?</t>
+  </si>
+  <si>
+    <t>What are the guidelines for the use of immuntherapy or targeted therapy in cervical cancer treatment, particularly for advanced or recurrent case?</t>
+  </si>
+  <si>
+    <t>Welche Leitlinien gibt es zum Einsatz von Immuntherapie oder zielgerichteter Therapie bei der Behandlung des Zervixkarzinoms, insbesondere bei fortgeschrittenen oder rezidivierten Fällen?</t>
+  </si>
+  <si>
+    <t>What are the current screening recommendations for cervical cancer, and how often should women undergo screening based on age and risk factors?</t>
+  </si>
+  <si>
+    <t>Was sind die aktuellen Screening-Empfehlungen für das Zervixkarzinom, und wie oft sollten Frauen je nach Alter und Risikofaktoren untersucht werden?</t>
+  </si>
+  <si>
+    <t>What are the preferred treatment modalities for early-stage laryngeal carcinoma (stages I and II)?</t>
+  </si>
+  <si>
+    <t>Welche bevorzugten Therapieoptionen gibt es für das Larynxkarzinom im Frühstadium (Stadien I und II)?</t>
+  </si>
+  <si>
+    <t>When is chemotherapy recommended as part of the treatmen ploan for advanced stage laryngeal carcinome(stages III and IV)?</t>
+  </si>
+  <si>
+    <t>Wann wird eine Chemotherapie als Teil des Behandlungsplans für das fortgeschrittene Larynxkarzinom (Stadien III und IV) empfohlen?</t>
+  </si>
+  <si>
+    <t>What are the recommended first-line investigations for detecting the primary tumor in cervical CUP cases?</t>
+  </si>
+  <si>
+    <t>Welche empfohlenen Erstuntersuchungen gibt es zum Nachweis des Primärtumors bei CUP-Fällen mit zervikalen Lymphknotenmetastasen?</t>
+  </si>
+  <si>
+    <t>What are the standard cirteria for classifying uterine soft tissue sarcomas?</t>
+  </si>
+  <si>
+    <t>Was sind die Standardkriterien zur Klassifikation uteriner Weichteilsarkome?</t>
+  </si>
+  <si>
+    <t>How are uterine soft tissue sarcomas generally classified?</t>
+  </si>
+  <si>
+    <t>Wie werden uterine Weichteilsarkome allgemein eingeteilt?</t>
+  </si>
+  <si>
+    <t>What are the diagnostic criteria for identifying neuroendocrine tumors in the bone?</t>
+  </si>
+  <si>
+    <t>Welche diagnostischen Kriterien gibt es zur Identifikation neuroendokriner Tumoren des Knochens?</t>
+  </si>
+  <si>
+    <t>What are the current treatment options for neuroendocrine tumors in the bone?</t>
+  </si>
+  <si>
+    <t>Was sind die aktuellen Therapieoptionen für neuroendokrine Tumoren des Knochens?</t>
+  </si>
+  <si>
+    <t>How are neuroendocrine tumors of the bone managed in terms of surgical intervention and medical therapy?</t>
+  </si>
+  <si>
+    <t>Wie werden neuroendokrine Knochentumoren hinsichtlich chirurgischer Intervention und medikamentöser Therapie behandelt?</t>
+  </si>
+  <si>
+    <t>What were the findings of the GORTEC 2007-02 study regarding induction chemotherapy for hypopharyngeal cancer?</t>
+  </si>
+  <si>
+    <t>Welche Ergebnisse zeigte die GORTEC-2007-02-Studie zur Induktionschemotherapie beim Hypopharynxkarzinom?</t>
+  </si>
+  <si>
+    <t>Is induction chemotherapy followed by cetuximab and radiotherapy more effective than primary radiochemotherapy?</t>
+  </si>
+  <si>
+    <t>Ist eine Induktionschemotherapie, gefolgt von Cetuximab und Radiotherapie, wirksamer als eine primäre Radiochemotherapie?</t>
+  </si>
+  <si>
+    <t>This is somehow difficult, becuase depends on many foactor and also on the surgeons preference. OncoproAI is not really the tool for this (Although we do mention factors that should be considered).</t>
   </si>
   <si>
     <t>What is the standard classification of uterine soft tissue sarcomas?</t>
@@ -101,7 +267,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -109,9 +275,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Aptos Narrow&quot;"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,12 +310,21 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -144,6 +335,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -351,7 +546,256 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="69.13"/>
+    <col customWidth="1" min="1" max="1" width="121.25"/>
+    <col customWidth="1" min="2" max="2" width="111.5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2"/>
+      <c r="D29" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="82.38"/>
     <col customWidth="1" min="2" max="2" width="101.38"/>
   </cols>
   <sheetData>
@@ -364,107 +808,107 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+      <c r="A2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
+      <c r="A3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
+      <c r="A4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
+      <c r="A5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
+      <c r="A6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
+      <c r="A7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
+      <c r="A8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
+      <c r="A9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
+      <c r="A10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
+      <c r="A11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
+      <c r="A12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
+      <c r="A13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
+      <c r="A14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>